<commit_message>
changed project plan due to unforseen obstacles
</commit_message>
<xml_diff>
--- a/Code Louisville Project Plan.xlsx
+++ b/Code Louisville Project Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chato\Documents\SweetDefeat\SweetDefeat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AA9A2E1-F87E-4ACA-AB23-3AF0230AF65E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08199182-00E0-4842-8BFA-C60711369846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Timestamp</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>htaylor0102@kctcs.edu</t>
+  </si>
+  <si>
+    <t>(edited) Can't use coupons due to being in test mode on Stripe. Switched to just javascript and JSON and cookies. Also can't show stock due to being in testing mode on Stripe</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -382,7 +385,9 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>

</xml_diff>